<commit_message>
Updates to the paper tables
</commit_message>
<xml_diff>
--- a/reports/paper_tables.xlsx
+++ b/reports/paper_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/Dev/cotwins-analyses/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2C6673-B2DC-864A-9343-1E7AD93EB8BB}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D44BB495-BC3E-334D-B472-973F64CA1CE3}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30080" windowHeight="31760" activeTab="1" xr2:uid="{44479B8E-EB5C-B24C-9174-6213C5FD65FC}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30080" windowHeight="31760" xr2:uid="{44479B8E-EB5C-B24C-9174-6213C5FD65FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Table S1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="124">
   <si>
     <t>In-Person Assessments</t>
   </si>
@@ -289,9 +289,6 @@
     <t>Standard assessment of parental monitoring</t>
   </si>
   <si>
-    <t>Peer Engagement</t>
-  </si>
-  <si>
     <t>Assessment of twin's relationship with their friends</t>
   </si>
   <si>
@@ -408,6 +405,12 @@
   </si>
   <si>
     <t>When a twin tweets</t>
+  </si>
+  <si>
+    <t>AddHealth: Extracurricular Activities</t>
+  </si>
+  <si>
+    <t>Peer Involvement/Engagement</t>
   </si>
 </sst>
 </file>
@@ -439,7 +442,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -621,11 +624,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -644,6 +658,79 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -659,78 +746,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1046,10 +1069,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7220148D-8F24-C547-BCF3-1F96D7118ABB}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1069,7 +1092,7 @@
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -1080,324 +1103,348 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="24" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="19" t="s">
+      <c r="A5" s="34"/>
+      <c r="B5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="25" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="24" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A7" s="11"/>
+      <c r="A7" s="36"/>
       <c r="B7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="D7" s="31" t="s">
+      <c r="C7" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="26" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="26" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A9" s="11"/>
+      <c r="A9" s="36"/>
       <c r="B9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="31"/>
+      <c r="D9" s="26"/>
     </row>
     <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A10" s="11"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="31"/>
+      <c r="D10" s="26"/>
     </row>
     <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A11" s="11"/>
+      <c r="A11" s="36"/>
       <c r="B11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="26" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A12" s="11"/>
+      <c r="A12" s="36"/>
       <c r="B12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="26" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A13" s="11"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="26" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="7" t="s">
+    <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A14" s="36"/>
+      <c r="B14" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="38" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="37"/>
+      <c r="B15" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C15" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D15" s="25" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
+    <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A16" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B16" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C16" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="32" t="s">
+      <c r="D16" s="27" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A16" s="11"/>
-      <c r="B16" s="6" t="s">
+    <row r="17" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A17" s="36"/>
+      <c r="B17" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C17" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D17" s="26" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="11"/>
-      <c r="B17" s="5" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="36"/>
+      <c r="B18" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C18" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D18" s="26" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="25" t="s">
+    <row r="19" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19" s="36"/>
+      <c r="B19" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="37"/>
+      <c r="B20" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C20" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="30" t="s">
+      <c r="D20" s="39" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="11" t="s">
+    <row r="21" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B21" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C21" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="29"/>
-    </row>
-    <row r="20" spans="1:4" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="20" t="s">
+      <c r="D21" s="24"/>
+    </row>
+    <row r="22" spans="1:4" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="37"/>
+      <c r="B22" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="C22" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="30"/>
-    </row>
-    <row r="21" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
+      <c r="D22" s="25"/>
+    </row>
+    <row r="23" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A23" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B23" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="C23" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="29" t="s">
+      <c r="D23" s="24" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A22" s="11"/>
-      <c r="B22" s="5" t="s">
+    <row r="24" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A24" s="36"/>
+      <c r="B24" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="C24" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="31" t="s">
+      <c r="D24" s="26" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="11"/>
-      <c r="B23" s="27" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="36"/>
+      <c r="B25" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C25" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D25" s="26" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A24" s="11"/>
-      <c r="B24" s="22" t="s">
+    <row r="26" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A26" s="36"/>
+      <c r="B26" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="23" t="s">
+      <c r="C26" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="31" t="s">
+      <c r="D26" s="26" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A25" s="11"/>
-      <c r="B25" s="23" t="s">
+    <row r="27" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A27" s="36"/>
+      <c r="B27" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C27" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="31" t="s">
+      <c r="D27" s="26" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A26" s="11"/>
-      <c r="B26" s="22" t="s">
+    <row r="28" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A28" s="36"/>
+      <c r="B28" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="23" t="s">
+      <c r="C28" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="31"/>
-    </row>
-    <row r="27" spans="1:4" ht="112" x14ac:dyDescent="0.2">
-      <c r="A27" s="11"/>
-      <c r="B27" s="27" t="s">
+      <c r="D28" s="26"/>
+    </row>
+    <row r="29" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+      <c r="A29" s="36"/>
+      <c r="B29" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="27" t="s">
+      <c r="C29" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="31" t="s">
+      <c r="D29" s="26" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="11"/>
-      <c r="B28" s="23" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="36"/>
+      <c r="B30" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C30" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D28" s="31" t="s">
+      <c r="D30" s="26" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
-      <c r="B29" s="25" t="s">
+    <row r="31" spans="1:4" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="37"/>
+      <c r="B31" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="26" t="s">
+      <c r="C31" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="30" t="s">
+      <c r="D31" s="25" t="s">
         <v>67</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A29"/>
+    <mergeCell ref="A6:A15"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1408,8 +1455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66CD5AE4-E8E5-5E49-A82D-4A7092502AD0}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1427,10 +1474,10 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -1444,448 +1491,448 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A5" s="36"/>
+      <c r="B5" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A6" s="36"/>
+      <c r="B6" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" s="36"/>
+      <c r="B7" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" s="36"/>
+      <c r="B8" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A9" s="36"/>
+      <c r="B9" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="36"/>
+      <c r="B10" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A11" s="36"/>
+      <c r="B11" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" s="18" t="s">
+      <c r="C11" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="E11" s="18" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A5" s="11"/>
-      <c r="B5" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="E5" s="31" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" s="11"/>
-      <c r="B6" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="E6" s="23" t="s">
+    <row r="12" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A12" s="36"/>
+      <c r="B12" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12" s="18"/>
+    </row>
+    <row r="13" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A13" s="36"/>
+      <c r="B13" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" s="18" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="11"/>
-      <c r="B7" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
-      <c r="B8" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="E8" s="23" t="s">
+    <row r="14" spans="1:5" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="37"/>
+      <c r="B14" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="20" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A9" s="11"/>
-      <c r="B9" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="E9" s="31" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A10" s="11"/>
-      <c r="B10" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="E10" s="31" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A11" s="11"/>
-      <c r="B11" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="C11" s="22" t="s">
+    <row r="15" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A15" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="E15" s="29"/>
+    </row>
+    <row r="16" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A16" s="36"/>
+      <c r="B16" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="E16" s="22"/>
+    </row>
+    <row r="17" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="37"/>
+      <c r="B17" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="E17" s="20"/>
+    </row>
+    <row r="18" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A18" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="D11" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="E11" s="23" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A12" s="11"/>
-      <c r="B12" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="E12" s="23"/>
-    </row>
-    <row r="13" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A13" s="11"/>
-      <c r="B13" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="D13" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="E14" s="25" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="B15" s="34" t="s">
-        <v>102</v>
-      </c>
-      <c r="C15" s="34" t="s">
-        <v>103</v>
-      </c>
-      <c r="D15" s="34" t="s">
-        <v>106</v>
-      </c>
-      <c r="E15" s="34"/>
-    </row>
-    <row r="16" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A16" s="11"/>
-      <c r="B16" s="27" t="s">
-        <v>104</v>
-      </c>
-      <c r="C16" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="D16" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="E16" s="27"/>
-    </row>
-    <row r="17" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="25" t="s">
-        <v>108</v>
-      </c>
-      <c r="C17" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="D17" s="25" t="s">
+      <c r="B18" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="E17" s="25"/>
-    </row>
-    <row r="18" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="B18" s="18" t="s">
+      <c r="C18" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D18" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="E18" s="13"/>
+    </row>
+    <row r="19" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A19" s="36"/>
+      <c r="B19" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="D18" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="E18" s="18"/>
-    </row>
-    <row r="19" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A19" s="11"/>
-      <c r="B19" s="23" t="s">
+      <c r="C19" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="D19" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="E19" s="18"/>
+    </row>
+    <row r="20" spans="1:5" ht="81" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="37"/>
+      <c r="B20" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="D19" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="E19" s="23"/>
-    </row>
-    <row r="20" spans="1:5" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="25" t="s">
+      <c r="C20" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="D20" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="D20" s="25" t="s">
+      <c r="E20" s="20"/>
+    </row>
+    <row r="21" spans="1:5" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="E20" s="25"/>
-    </row>
-    <row r="21" spans="1:5" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="37" t="s">
+      <c r="B21" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="B21" s="36" t="s">
+      <c r="C21" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="C21" s="36" t="s">
+      <c r="D21" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="D21" s="36" t="s">
-        <v>122</v>
-      </c>
-      <c r="E21" s="36"/>
+      <c r="E21" s="31"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
-      <c r="B28" s="33"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
-      <c r="B29" s="33"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
-      <c r="B32" s="33"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
-      <c r="B33" s="33"/>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
-      <c r="B34" s="33"/>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
-      <c r="B35" s="33"/>
-      <c r="C35" s="33"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="28"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
-      <c r="B36" s="33"/>
-      <c r="C36" s="33"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="33"/>
+      <c r="B36" s="28"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="28"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
-      <c r="B37" s="33"/>
-      <c r="C37" s="33"/>
-      <c r="D37" s="33"/>
-      <c r="E37" s="33"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="28"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
-      <c r="B38" s="33"/>
-      <c r="C38" s="33"/>
-      <c r="D38" s="33"/>
-      <c r="E38" s="33"/>
+      <c r="B38" s="28"/>
+      <c r="C38" s="28"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="28"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
-      <c r="B39" s="33"/>
-      <c r="C39" s="33"/>
-      <c r="D39" s="33"/>
-      <c r="E39" s="33"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="28"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
-      <c r="B40" s="33"/>
-      <c r="C40" s="33"/>
-      <c r="D40" s="33"/>
-      <c r="E40" s="33"/>
+      <c r="B40" s="28"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="28"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
-      <c r="B41" s="33"/>
-      <c r="C41" s="33"/>
-      <c r="D41" s="33"/>
-      <c r="E41" s="33"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="28"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
-      <c r="B42" s="33"/>
-      <c r="C42" s="33"/>
-      <c r="D42" s="33"/>
-      <c r="E42" s="33"/>
+      <c r="B42" s="28"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="28"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
-      <c r="B43" s="33"/>
-      <c r="C43" s="33"/>
-      <c r="D43" s="33"/>
-      <c r="E43" s="33"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="28"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
-      <c r="B44" s="33"/>
-      <c r="C44" s="33"/>
-      <c r="D44" s="33"/>
-      <c r="E44" s="33"/>
+      <c r="B44" s="28"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="28"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
-      <c r="B45" s="33"/>
-      <c r="C45" s="33"/>
-      <c r="D45" s="33"/>
-      <c r="E45" s="33"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="28"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
-      <c r="B46" s="33"/>
-      <c r="C46" s="33"/>
-      <c r="D46" s="33"/>
-      <c r="E46" s="33"/>
+      <c r="B46" s="28"/>
+      <c r="C46" s="28"/>
+      <c r="D46" s="28"/>
+      <c r="E46" s="28"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
-      <c r="B47" s="33"/>
-      <c r="C47" s="33"/>
-      <c r="D47" s="33"/>
-      <c r="E47" s="33"/>
+      <c r="B47" s="28"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="28"/>
+      <c r="E47" s="28"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="2"/>

</xml_diff>

<commit_message>
Updating the plots for the latex SI
</commit_message>
<xml_diff>
--- a/reports/paper_tables.xlsx
+++ b/reports/paper_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/Dev/cotwins-analyses/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D028F371-EC91-994E-86E9-16952B8B0870}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E1D0A3-9D23-0F47-B13C-8B737D58A5D9}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30080" windowHeight="31760" activeTab="1" xr2:uid="{44479B8E-EB5C-B24C-9174-6213C5FD65FC}"/>
+    <workbookView xWindow="30080" yWindow="460" windowWidth="30080" windowHeight="31760" activeTab="1" xr2:uid="{44479B8E-EB5C-B24C-9174-6213C5FD65FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Table S1" sheetId="1" r:id="rId1"/>
@@ -26,13 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="126">
-  <si>
-    <t>In-Person Assessments</t>
-  </si>
-  <si>
-    <t>Remote Assessments</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="132">
   <si>
     <t>Type</t>
   </si>
@@ -235,9 +229,6 @@
     <t>Frequency</t>
   </si>
   <si>
-    <t>Weekly (with a random offset)</t>
-  </si>
-  <si>
     <t>Friedman, 2016</t>
   </si>
   <si>
@@ -247,9 +238,6 @@
     <t>Measurement of recent substance use quantity and frequency</t>
   </si>
   <si>
-    <t>Every six weeks</t>
-  </si>
-  <si>
     <t>Assessment of twin's extracurricular activities</t>
   </si>
   <si>
@@ -265,15 +253,9 @@
     <t>Life Events</t>
   </si>
   <si>
-    <t>Monthly</t>
-  </si>
-  <si>
     <t>Parental Monitoring</t>
   </si>
   <si>
-    <t>Every two months</t>
-  </si>
-  <si>
     <t>Standard assessment of parental monitoring</t>
   </si>
   <si>
@@ -290,9 +272,6 @@
   </si>
   <si>
     <t>Standard Big Five measure of personality</t>
-  </si>
-  <si>
-    <t>Every six months</t>
   </si>
   <si>
     <t>Social Media Use</t>
@@ -417,6 +396,50 @@
   </si>
   <si>
     <t>Developed for this study</t>
+  </si>
+  <si>
+    <t>Initially: Every 5±2 days
+After 5/8/17: Every 7±2 days</t>
+  </si>
+  <si>
+    <t>Every 170±6 days</t>
+  </si>
+  <si>
+    <t>Every 30±5 days</t>
+  </si>
+  <si>
+    <t>Every 60±10 days</t>
+  </si>
+  <si>
+    <t>Every 25±3 days</t>
+  </si>
+  <si>
+    <t>Every 30±10 days</t>
+  </si>
+  <si>
+    <t>Initially: Every 180±3 days
+After 3/24/17: Every 300±3 days</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Keep Track (Updating)
+Category Shift (Switching)</t>
+  </si>
+  <si>
+    <t>Browser-based assessments of executive function</t>
+  </si>
+  <si>
+    <t>Every 300 days</t>
+  </si>
+  <si>
+    <t>Initially: Every 40±3 days
+After 11/3/17: Every 100±3 days</t>
+  </si>
+  <si>
+    <t>Conway, 2014
+Hamilton, 2011</t>
   </si>
 </sst>
 </file>
@@ -645,9 +668,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -742,20 +764,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1071,386 +1093,383 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7220148D-8F24-C547-BCF3-1F96D7118ABB}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="D1" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A2" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D2" s="22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="37"/>
+      <c r="B3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>122</v>
+      <c r="D3" s="23" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A5" s="34"/>
+      <c r="B5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A6" s="34"/>
+      <c r="B6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="23" t="s">
+      <c r="D6" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" s="34"/>
+      <c r="B7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" s="34"/>
+      <c r="B8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A9" s="34"/>
+      <c r="B9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="34"/>
+      <c r="B10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" s="34"/>
+      <c r="B11" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="35"/>
+      <c r="B12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A13" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="25" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35"/>
-      <c r="B5" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="24" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A7" s="37"/>
-      <c r="B7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A8" s="37"/>
-      <c r="B8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A9" s="37"/>
-      <c r="B9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A10" s="37"/>
-      <c r="B10" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A11" s="37"/>
-      <c r="B11" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A12" s="37"/>
-      <c r="B12" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A13" s="37"/>
-      <c r="B13" s="33" t="s">
-        <v>123</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="D13" s="31" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="38"/>
-      <c r="B14" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>24</v>
+    <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A14" s="34"/>
+      <c r="B14" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>27</v>
       </c>
       <c r="D14" s="24" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A15" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="18" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="34"/>
+      <c r="B15" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A16" s="34"/>
+      <c r="B16" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="35"/>
+      <c r="B17" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="26" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A16" s="37"/>
-      <c r="B16" s="16" t="s">
+      <c r="D17" s="31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="22"/>
+    </row>
+    <row r="19" spans="1:4" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="35"/>
+      <c r="B19" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="23"/>
+    </row>
+    <row r="20" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A20" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A21" s="34"/>
+      <c r="B21" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="34"/>
+      <c r="B22" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A23" s="34"/>
+      <c r="B23" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A24" s="34"/>
+      <c r="B24" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A25" s="34"/>
+      <c r="B25" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+      <c r="A26" s="34"/>
+      <c r="B26" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="34"/>
+      <c r="B27" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C27" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="37"/>
-      <c r="B17" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A18" s="37"/>
-      <c r="B18" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="38"/>
-      <c r="B19" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="23"/>
-    </row>
-    <row r="21" spans="1:4" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="38"/>
-      <c r="B21" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="24"/>
-    </row>
-    <row r="22" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A22" s="36" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" s="23" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A23" s="37"/>
-      <c r="B23" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" s="25" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="37"/>
-      <c r="B24" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="25" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A25" s="37"/>
-      <c r="B25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A26" s="37"/>
-      <c r="B26" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" s="25" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A27" s="37"/>
-      <c r="B27" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" s="25"/>
-    </row>
-    <row r="28" spans="1:4" ht="112" x14ac:dyDescent="0.2">
-      <c r="A28" s="37"/>
-      <c r="B28" s="21" t="s">
+      <c r="D27" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="35"/>
+      <c r="B28" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="C28" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="D28" s="25" t="s">
+      <c r="D28" s="23" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="37"/>
-      <c r="B29" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29" s="25" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="38"/>
-      <c r="B30" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="D30" s="24" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A6:A14"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A30"/>
-    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A28"/>
+    <mergeCell ref="A2:A3"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="7" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66CD5AE4-E8E5-5E49-A82D-4A7092502AD0}">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1462,505 +1481,511 @@
     <col min="5" max="5" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="D1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A2" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" s="34"/>
+      <c r="B3" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A4" s="34"/>
+      <c r="B4" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A5" s="34"/>
+      <c r="B5" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A6" s="34"/>
+      <c r="B6" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="C6" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" s="34"/>
+      <c r="B7" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="16" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A4" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="12" t="s">
+      <c r="E7" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A8" s="34"/>
+      <c r="B8" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A9" s="34"/>
+      <c r="B9" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A10" s="34"/>
+      <c r="B10" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" s="34"/>
+      <c r="B11" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="35"/>
+      <c r="B12" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A13" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" s="27"/>
+    </row>
+    <row r="14" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A14" s="34"/>
+      <c r="B14" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A5" s="37"/>
-      <c r="B5" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="E5" s="25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A6" s="37"/>
-      <c r="B6" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="37"/>
-      <c r="B7" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" s="37"/>
-      <c r="B8" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A9" s="37"/>
-      <c r="B9" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="E9" s="25" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A10" s="37"/>
-      <c r="B10" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A11" s="37"/>
-      <c r="B11" s="17" t="s">
+      <c r="C14" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="C11" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A12" s="37"/>
-      <c r="B12" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="D12" s="17" t="s">
+      <c r="D14" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="16"/>
+    </row>
+    <row r="15" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="35"/>
+      <c r="B15" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="E15" s="13"/>
+    </row>
+    <row r="16" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A16" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="E12" s="17" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A13" s="37"/>
-      <c r="B13" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="38"/>
-      <c r="B14" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A15" s="36" t="s">
-        <v>96</v>
-      </c>
-      <c r="B15" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="C15" s="28" t="s">
-        <v>98</v>
-      </c>
-      <c r="D15" s="28" t="s">
+      <c r="B16" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="E15" s="28"/>
-    </row>
-    <row r="16" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A16" s="37"/>
-      <c r="B16" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="C16" s="21" t="s">
+      <c r="D16" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="E16" s="11"/>
+    </row>
+    <row r="17" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A17" s="34"/>
+      <c r="B17" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="E16" s="21"/>
-    </row>
-    <row r="17" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="38"/>
-      <c r="B17" s="19" t="s">
+      <c r="C17" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="D17" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="E17" s="16"/>
+    </row>
+    <row r="18" spans="1:5" ht="81" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="35"/>
+      <c r="B18" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="C18" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="E17" s="19"/>
-    </row>
-    <row r="18" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A18" s="36" t="s">
-        <v>95</v>
-      </c>
-      <c r="B18" s="12" t="s">
+      <c r="D18" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="E18" s="13"/>
+    </row>
+    <row r="19" spans="1:5" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="B19" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="D18" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="E18" s="12"/>
-    </row>
-    <row r="19" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A19" s="37"/>
-      <c r="B19" s="17" t="s">
+      <c r="C19" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="D19" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="D19" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="E19" s="17"/>
-    </row>
-    <row r="20" spans="1:5" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="38"/>
-      <c r="B20" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="E20" s="19"/>
-    </row>
-    <row r="21" spans="1:5" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="B21" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="C21" s="29" t="s">
-        <v>116</v>
-      </c>
-      <c r="D21" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="E21" s="29"/>
+      <c r="E19" s="28"/>
+    </row>
+    <row r="20" spans="1:5" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
+      <c r="A22" s="1"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
+      <c r="A23" s="1"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="2"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
+      <c r="A24" s="1"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="2"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
+      <c r="A25" s="1"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="2"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
+      <c r="A26" s="1"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
+      <c r="A27" s="1"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
+      <c r="A28" s="1"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="2"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
+      <c r="A29" s="1"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
+      <c r="A30" s="1"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
+      <c r="A31" s="1"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
+      <c r="A32" s="1"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="2"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
+      <c r="A33" s="1"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
+      <c r="A34" s="1"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
-      <c r="B35" s="27"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="27"/>
+      <c r="A35" s="1"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="2"/>
-      <c r="B36" s="27"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="27"/>
+      <c r="A36" s="1"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="2"/>
-      <c r="B37" s="27"/>
-      <c r="C37" s="27"/>
-      <c r="D37" s="27"/>
-      <c r="E37" s="27"/>
+      <c r="A37" s="1"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="2"/>
-      <c r="B38" s="27"/>
-      <c r="C38" s="27"/>
-      <c r="D38" s="27"/>
-      <c r="E38" s="27"/>
+      <c r="A38" s="1"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="2"/>
-      <c r="B39" s="27"/>
-      <c r="C39" s="27"/>
-      <c r="D39" s="27"/>
-      <c r="E39" s="27"/>
+      <c r="A39" s="1"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="2"/>
-      <c r="B40" s="27"/>
-      <c r="C40" s="27"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="27"/>
+      <c r="A40" s="1"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="2"/>
-      <c r="B41" s="27"/>
-      <c r="C41" s="27"/>
-      <c r="D41" s="27"/>
-      <c r="E41" s="27"/>
+      <c r="A41" s="1"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="2"/>
-      <c r="B42" s="27"/>
-      <c r="C42" s="27"/>
-      <c r="D42" s="27"/>
-      <c r="E42" s="27"/>
+      <c r="A42" s="1"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="2"/>
-      <c r="B43" s="27"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="27"/>
-      <c r="E43" s="27"/>
+      <c r="A43" s="1"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="2"/>
-      <c r="B44" s="27"/>
-      <c r="C44" s="27"/>
-      <c r="D44" s="27"/>
-      <c r="E44" s="27"/>
+      <c r="A44" s="1"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="26"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="2"/>
-      <c r="B45" s="27"/>
-      <c r="C45" s="27"/>
-      <c r="D45" s="27"/>
-      <c r="E45" s="27"/>
+      <c r="A45" s="1"/>
+      <c r="B45" s="26"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="26"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="2"/>
-      <c r="B46" s="27"/>
-      <c r="C46" s="27"/>
-      <c r="D46" s="27"/>
-      <c r="E46" s="27"/>
+      <c r="A46" s="1"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="2"/>
-      <c r="B47" s="27"/>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="27"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="2"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A4:A14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A2:A12"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A16:A18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added a table of substance use and dependence at intake
</commit_message>
<xml_diff>
--- a/reports/paper_tables.xlsx
+++ b/reports/paper_tables.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/Dev/cotwins-analyses/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E1D0A3-9D23-0F47-B13C-8B737D58A5D9}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51261DB4-37B0-E64C-B4FF-01905A8260BA}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30080" yWindow="460" windowWidth="30080" windowHeight="31760" activeTab="1" xr2:uid="{44479B8E-EB5C-B24C-9174-6213C5FD65FC}"/>
+    <workbookView xWindow="4060" yWindow="5920" windowWidth="28500" windowHeight="15880" xr2:uid="{44479B8E-EB5C-B24C-9174-6213C5FD65FC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Table S1" sheetId="1" r:id="rId1"/>
-    <sheet name="Table S2" sheetId="2" r:id="rId2"/>
+    <sheet name="Table 1" sheetId="3" r:id="rId1"/>
+    <sheet name="Table S1" sheetId="1" r:id="rId2"/>
+    <sheet name="Table S2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="163">
   <si>
     <t>Type</t>
   </si>
@@ -440,6 +441,99 @@
   <si>
     <t>Conway, 2014
 Hamilton, 2011</t>
+  </si>
+  <si>
+    <t>Alcohol</t>
+  </si>
+  <si>
+    <t>Marijuana</t>
+  </si>
+  <si>
+    <t>Cigarettes</t>
+  </si>
+  <si>
+    <t>Current user</t>
+  </si>
+  <si>
+    <t>Ever used</t>
+  </si>
+  <si>
+    <t>HKCS Ever used</t>
+  </si>
+  <si>
+    <t>HKCS Current user</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>38.0</t>
+  </si>
+  <si>
+    <t>21.2</t>
+  </si>
+  <si>
+    <t>Cocaine</t>
+  </si>
+  <si>
+    <t>5.6</t>
+  </si>
+  <si>
+    <t>Heroin</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>20.0</t>
+  </si>
+  <si>
+    <t>59.2</t>
+  </si>
+  <si>
+    <t>0.9</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>37.9</t>
+  </si>
+  <si>
+    <t>16.6</t>
+  </si>
+  <si>
+    <t>0.4</t>
+  </si>
+  <si>
+    <t>6.4</t>
+  </si>
+  <si>
+    <t>13.3</t>
+  </si>
+  <si>
+    <t>HKCS = Healthy Kids Colorado Survey</t>
+  </si>
+  <si>
+    <t>1.2 (All tobacco)</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>4.5</t>
+  </si>
+  <si>
+    <t>Maximum age at recruitment = 18, so some loss of oldest high school kids</t>
+  </si>
+  <si>
+    <t>Median family income is $100,000-$150,000, Median household income in Colorado is $62,520 (2016 American Community Survey)</t>
+  </si>
+  <si>
+    <t>62.1% of the parents who responded have a bachelor's degree or higher, 38.7% of those 25 years or older in Colorado have a bachelor's degree or higher (2016 American Community Survey)</t>
+  </si>
+  <si>
+    <t>Dependence in last year</t>
   </si>
 </sst>
 </file>
@@ -668,7 +762,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -779,6 +873,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1092,6 +1187,165 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D88095D-9956-6043-97F5-2A76D09352F9}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2" s="38">
+        <v>30.2</v>
+      </c>
+      <c r="F2" s="38" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>140</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>153</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="F3" s="38" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>152</v>
+      </c>
+      <c r="E4" s="38">
+        <v>8.6</v>
+      </c>
+      <c r="F4" s="38" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>143</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>149</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>139</v>
+      </c>
+      <c r="F5" s="38" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>149</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>149</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>139</v>
+      </c>
+      <c r="F6" s="38" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7220148D-8F24-C547-BCF3-1F96D7118ABB}">
   <dimension ref="A1:D28"/>
   <sheetViews>
@@ -1464,11 +1718,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66CD5AE4-E8E5-5E49-A82D-4A7092502AD0}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
More comments on table
</commit_message>
<xml_diff>
--- a/reports/paper_tables.xlsx
+++ b/reports/paper_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/Dev/cotwins-analyses/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51261DB4-37B0-E64C-B4FF-01905A8260BA}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950405E5-E01D-6940-9BA1-402E7E33AE12}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4060" yWindow="5920" windowWidth="28500" windowHeight="15880" xr2:uid="{44479B8E-EB5C-B24C-9174-6213C5FD65FC}"/>
+    <workbookView xWindow="30080" yWindow="460" windowWidth="30080" windowHeight="31760" xr2:uid="{44479B8E-EB5C-B24C-9174-6213C5FD65FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="165">
   <si>
     <t>Type</t>
   </si>
@@ -524,9 +524,6 @@
     <t>4.5</t>
   </si>
   <si>
-    <t>Maximum age at recruitment = 18, so some loss of oldest high school kids</t>
-  </si>
-  <si>
     <t>Median family income is $100,000-$150,000, Median household income in Colorado is $62,520 (2016 American Community Survey)</t>
   </si>
   <si>
@@ -534,6 +531,15 @@
   </si>
   <si>
     <t>Dependence in last year</t>
+  </si>
+  <si>
+    <t>Maximum age at recruitment = 18, so some loss of oldest high school kids and some 14 year old still in 8th grade</t>
+  </si>
+  <si>
+    <t>Requirement to have phones</t>
+  </si>
+  <si>
+    <t>Must be native born coloradan to be in birth records and in twin registry</t>
   </si>
 </sst>
 </file>
@@ -858,6 +864,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -873,7 +880,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1188,10 +1194,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D88095D-9956-6043-97F5-2A76D09352F9}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1217,26 +1223,26 @@
         <v>138</v>
       </c>
       <c r="F1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>132</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="33" t="s">
         <v>154</v>
       </c>
-      <c r="E2" s="38">
+      <c r="E2" s="33">
         <v>30.2</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="33" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1244,19 +1250,19 @@
       <c r="A3" t="s">
         <v>133</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="33" t="s">
         <v>153</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="33" t="s">
         <v>157</v>
       </c>
     </row>
@@ -1264,19 +1270,19 @@
       <c r="A4" t="s">
         <v>134</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="33" t="s">
         <v>152</v>
       </c>
-      <c r="E4" s="38">
+      <c r="E4" s="33">
         <v>8.6</v>
       </c>
-      <c r="F4" s="38" t="s">
+      <c r="F4" s="33" t="s">
         <v>156</v>
       </c>
     </row>
@@ -1284,39 +1290,39 @@
       <c r="A5" t="s">
         <v>142</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="33" t="s">
         <v>143</v>
       </c>
-      <c r="D5" s="38" t="s">
+      <c r="D5" s="33" t="s">
         <v>149</v>
       </c>
-      <c r="E5" s="38" t="s">
+      <c r="E5" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="F5" s="38" t="s">
+      <c r="F5" s="33" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="33" t="s">
         <v>149</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="33" t="s">
         <v>149</v>
       </c>
-      <c r="E6" s="38" t="s">
+      <c r="E6" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="F6" s="38" t="s">
+      <c r="F6" s="33" t="s">
         <v>149</v>
       </c>
     </row>
@@ -1327,17 +1333,27 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>161</v>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -1376,7 +1392,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="37" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="10" t="s">
@@ -1390,7 +1406,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37"/>
+      <c r="A3" s="38"/>
       <c r="B3" s="12" t="s">
         <v>5</v>
       </c>
@@ -1402,7 +1418,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="34" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -1416,7 +1432,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A5" s="34"/>
+      <c r="A5" s="35"/>
       <c r="B5" s="4" t="s">
         <v>17</v>
       </c>
@@ -1428,7 +1444,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A6" s="34"/>
+      <c r="A6" s="35"/>
       <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
@@ -1440,7 +1456,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="34"/>
+      <c r="A7" s="35"/>
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
@@ -1452,7 +1468,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" s="34"/>
+      <c r="A8" s="35"/>
       <c r="B8" s="5" t="s">
         <v>16</v>
       </c>
@@ -1464,7 +1480,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A9" s="34"/>
+      <c r="A9" s="35"/>
       <c r="B9" s="5" t="s">
         <v>15</v>
       </c>
@@ -1476,7 +1492,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A10" s="34"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
@@ -1488,7 +1504,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A11" s="34"/>
+      <c r="A11" s="35"/>
       <c r="B11" s="32" t="s">
         <v>116</v>
       </c>
@@ -1500,7 +1516,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
+      <c r="A12" s="36"/>
       <c r="B12" s="6" t="s">
         <v>21</v>
       </c>
@@ -1512,7 +1528,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="34" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="17" t="s">
@@ -1526,7 +1542,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A14" s="34"/>
+      <c r="A14" s="35"/>
       <c r="B14" s="15" t="s">
         <v>26</v>
       </c>
@@ -1538,7 +1554,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="34"/>
+      <c r="A15" s="35"/>
       <c r="B15" s="16" t="s">
         <v>28</v>
       </c>
@@ -1550,7 +1566,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A16" s="34"/>
+      <c r="A16" s="35"/>
       <c r="B16" s="16" t="s">
         <v>111</v>
       </c>
@@ -1562,7 +1578,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
+      <c r="A17" s="36"/>
       <c r="B17" s="18" t="s">
         <v>31</v>
       </c>
@@ -1574,7 +1590,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="33" t="s">
+      <c r="A18" s="34" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="20" t="s">
@@ -1586,7 +1602,7 @@
       <c r="D18" s="22"/>
     </row>
     <row r="19" spans="1:4" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
+      <c r="A19" s="36"/>
       <c r="B19" s="13" t="s">
         <v>36</v>
       </c>
@@ -1596,7 +1612,7 @@
       <c r="D19" s="23"/>
     </row>
     <row r="20" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="34" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="11" t="s">
@@ -1610,7 +1626,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A21" s="34"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="16" t="s">
         <v>40</v>
       </c>
@@ -1622,7 +1638,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="34"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="20" t="s">
         <v>42</v>
       </c>
@@ -1634,7 +1650,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A23" s="34"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="15" t="s">
         <v>14</v>
       </c>
@@ -1646,7 +1662,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A24" s="34"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="16" t="s">
         <v>45</v>
       </c>
@@ -1658,7 +1674,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A25" s="34"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="15" t="s">
         <v>11</v>
       </c>
@@ -1670,7 +1686,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="112" x14ac:dyDescent="0.2">
-      <c r="A26" s="34"/>
+      <c r="A26" s="35"/>
       <c r="B26" s="20" t="s">
         <v>46</v>
       </c>
@@ -1682,7 +1698,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="34"/>
+      <c r="A27" s="35"/>
       <c r="B27" s="16" t="s">
         <v>28</v>
       </c>
@@ -1694,7 +1710,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="35"/>
+      <c r="A28" s="36"/>
       <c r="B28" s="18" t="s">
         <v>48</v>
       </c>
@@ -1753,7 +1769,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="35" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="11" t="s">
@@ -1770,7 +1786,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A3" s="34"/>
+      <c r="A3" s="35"/>
       <c r="B3" s="16" t="s">
         <v>71</v>
       </c>
@@ -1785,7 +1801,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A4" s="34"/>
+      <c r="A4" s="35"/>
       <c r="B4" s="16" t="s">
         <v>112</v>
       </c>
@@ -1800,7 +1816,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A5" s="34"/>
+      <c r="A5" s="35"/>
       <c r="B5" s="16" t="s">
         <v>75</v>
       </c>
@@ -1815,7 +1831,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A6" s="34"/>
+      <c r="A6" s="35"/>
       <c r="B6" s="16" t="s">
         <v>65</v>
       </c>
@@ -1830,7 +1846,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="34"/>
+      <c r="A7" s="35"/>
       <c r="B7" s="16" t="s">
         <v>72</v>
       </c>
@@ -1845,7 +1861,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A8" s="34"/>
+      <c r="A8" s="35"/>
       <c r="B8" s="16" t="s">
         <v>77</v>
       </c>
@@ -1860,7 +1876,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A9" s="34"/>
+      <c r="A9" s="35"/>
       <c r="B9" s="16" t="s">
         <v>86</v>
       </c>
@@ -1875,7 +1891,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A10" s="34"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="16" t="s">
         <v>79</v>
       </c>
@@ -1890,7 +1906,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A11" s="34"/>
+      <c r="A11" s="35"/>
       <c r="B11" s="16" t="s">
         <v>82</v>
       </c>
@@ -1905,7 +1921,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
+      <c r="A12" s="36"/>
       <c r="B12" s="18" t="s">
         <v>68</v>
       </c>
@@ -1920,7 +1936,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="34" t="s">
         <v>89</v>
       </c>
       <c r="B13" s="27" t="s">
@@ -1935,7 +1951,7 @@
       <c r="E13" s="27"/>
     </row>
     <row r="14" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A14" s="34"/>
+      <c r="A14" s="35"/>
       <c r="B14" s="4" t="s">
         <v>92</v>
       </c>
@@ -1948,7 +1964,7 @@
       <c r="E14" s="16"/>
     </row>
     <row r="15" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35"/>
+      <c r="A15" s="36"/>
       <c r="B15" s="12" t="s">
         <v>96</v>
       </c>
@@ -1961,7 +1977,7 @@
       <c r="E15" s="13"/>
     </row>
     <row r="16" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="34" t="s">
         <v>88</v>
       </c>
       <c r="B16" s="11" t="s">
@@ -1976,7 +1992,7 @@
       <c r="E16" s="11"/>
     </row>
     <row r="17" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A17" s="34"/>
+      <c r="A17" s="35"/>
       <c r="B17" s="16" t="s">
         <v>102</v>
       </c>
@@ -1989,7 +2005,7 @@
       <c r="E17" s="16"/>
     </row>
     <row r="18" spans="1:5" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
+      <c r="A18" s="36"/>
       <c r="B18" s="12" t="s">
         <v>104</v>
       </c>

</xml_diff>

<commit_message>
Working on the tables for the paper
</commit_message>
<xml_diff>
--- a/reports/paper_tables.xlsx
+++ b/reports/paper_tables.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/Dev/cotwins-analyses/reports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Brazel\Dev\cotwins-analyses\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950405E5-E01D-6940-9BA1-402E7E33AE12}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30080" yWindow="460" windowWidth="30080" windowHeight="31760" xr2:uid="{44479B8E-EB5C-B24C-9174-6213C5FD65FC}"/>
+    <workbookView xWindow="30084" yWindow="456" windowWidth="30084" windowHeight="31764"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="3" r:id="rId1"/>
@@ -545,7 +544,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1193,23 +1192,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D88095D-9956-6043-97F5-2A76D09352F9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.796875" customWidth="1"/>
+    <col min="3" max="3" width="13.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>136</v>
       </c>
@@ -1226,7 +1225,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>132</v>
       </c>
@@ -1246,7 +1245,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>133</v>
       </c>
@@ -1266,7 +1265,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>134</v>
       </c>
@@ -1286,7 +1285,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>142</v>
       </c>
@@ -1306,7 +1305,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="33" t="s">
         <v>144</v>
       </c>
@@ -1326,32 +1325,32 @@
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>164</v>
       </c>
@@ -1362,22 +1361,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7220148D-8F24-C547-BCF3-1F96D7118ABB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1391,7 +1390,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A2" s="37" t="s">
         <v>8</v>
       </c>
@@ -1405,7 +1404,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="38"/>
       <c r="B3" s="12" t="s">
         <v>5</v>
@@ -1417,7 +1416,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A4" s="34" t="s">
         <v>9</v>
       </c>
@@ -1431,7 +1430,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="35"/>
       <c r="B5" s="4" t="s">
         <v>17</v>
@@ -1443,7 +1442,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A6" s="35"/>
       <c r="B6" s="4" t="s">
         <v>13</v>
@@ -1455,7 +1454,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A7" s="35"/>
       <c r="B7" s="5" t="s">
         <v>11</v>
@@ -1467,7 +1466,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A8" s="35"/>
       <c r="B8" s="5" t="s">
         <v>16</v>
@@ -1479,7 +1478,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A9" s="35"/>
       <c r="B9" s="5" t="s">
         <v>15</v>
@@ -1491,7 +1490,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A10" s="35"/>
       <c r="B10" s="5" t="s">
         <v>14</v>
@@ -1503,7 +1502,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A11" s="35"/>
       <c r="B11" s="32" t="s">
         <v>116</v>
@@ -1515,7 +1514,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="36"/>
       <c r="B12" s="6" t="s">
         <v>21</v>
@@ -1527,7 +1526,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A13" s="34" t="s">
         <v>24</v>
       </c>
@@ -1541,7 +1540,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="35"/>
       <c r="B14" s="15" t="s">
         <v>26</v>
@@ -1553,7 +1552,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="35"/>
       <c r="B15" s="16" t="s">
         <v>28</v>
@@ -1565,7 +1564,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A16" s="35"/>
       <c r="B16" s="16" t="s">
         <v>111</v>
@@ -1577,7 +1576,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="36"/>
       <c r="B17" s="18" t="s">
         <v>31</v>
@@ -1589,7 +1588,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="34" t="s">
         <v>33</v>
       </c>
@@ -1601,7 +1600,7 @@
       </c>
       <c r="D18" s="22"/>
     </row>
-    <row r="19" spans="1:4" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="31.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="36"/>
       <c r="B19" s="13" t="s">
         <v>36</v>
@@ -1611,7 +1610,7 @@
       </c>
       <c r="D19" s="23"/>
     </row>
-    <row r="20" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A20" s="34" t="s">
         <v>38</v>
       </c>
@@ -1625,7 +1624,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A21" s="35"/>
       <c r="B21" s="16" t="s">
         <v>40</v>
@@ -1637,7 +1636,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="35"/>
       <c r="B22" s="20" t="s">
         <v>42</v>
@@ -1649,7 +1648,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A23" s="35"/>
       <c r="B23" s="15" t="s">
         <v>14</v>
@@ -1661,7 +1660,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A24" s="35"/>
       <c r="B24" s="16" t="s">
         <v>45</v>
@@ -1673,7 +1672,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A25" s="35"/>
       <c r="B25" s="15" t="s">
         <v>11</v>
@@ -1685,7 +1684,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A26" s="35"/>
       <c r="B26" s="20" t="s">
         <v>46</v>
@@ -1697,7 +1696,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="35"/>
       <c r="B27" s="16" t="s">
         <v>28</v>
@@ -1709,7 +1708,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="36"/>
       <c r="B28" s="18" t="s">
         <v>48</v>
@@ -1735,23 +1734,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66CD5AE4-E8E5-5E49-A82D-4A7092502AD0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="22.1640625" customWidth="1"/>
-    <col min="3" max="3" width="26.83203125" customWidth="1"/>
-    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22.19921875" customWidth="1"/>
+    <col min="3" max="3" width="26.796875" customWidth="1"/>
+    <col min="4" max="4" width="24.296875" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1768,7 +1767,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
         <v>23</v>
       </c>
@@ -1785,7 +1784,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A3" s="35"/>
       <c r="B3" s="16" t="s">
         <v>71</v>
@@ -1800,7 +1799,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A4" s="35"/>
       <c r="B4" s="16" t="s">
         <v>112</v>
@@ -1815,7 +1814,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A5" s="35"/>
       <c r="B5" s="16" t="s">
         <v>75</v>
@@ -1830,7 +1829,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A6" s="35"/>
       <c r="B6" s="16" t="s">
         <v>65</v>
@@ -1845,7 +1844,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A7" s="35"/>
       <c r="B7" s="16" t="s">
         <v>72</v>
@@ -1860,7 +1859,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A8" s="35"/>
       <c r="B8" s="16" t="s">
         <v>77</v>
@@ -1875,7 +1874,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A9" s="35"/>
       <c r="B9" s="16" t="s">
         <v>86</v>
@@ -1890,7 +1889,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A10" s="35"/>
       <c r="B10" s="16" t="s">
         <v>79</v>
@@ -1905,7 +1904,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A11" s="35"/>
       <c r="B11" s="16" t="s">
         <v>82</v>
@@ -1920,7 +1919,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="63" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="36"/>
       <c r="B12" s="18" t="s">
         <v>68</v>
@@ -1935,7 +1934,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A13" s="34" t="s">
         <v>89</v>
       </c>
@@ -1950,7 +1949,7 @@
       </c>
       <c r="E13" s="27"/>
     </row>
-    <row r="14" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A14" s="35"/>
       <c r="B14" s="4" t="s">
         <v>92</v>
@@ -1963,7 +1962,7 @@
       </c>
       <c r="E14" s="16"/>
     </row>
-    <row r="15" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="36"/>
       <c r="B15" s="12" t="s">
         <v>96</v>
@@ -1976,7 +1975,7 @@
       </c>
       <c r="E15" s="13"/>
     </row>
-    <row r="16" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A16" s="34" t="s">
         <v>88</v>
       </c>
@@ -1991,7 +1990,7 @@
       </c>
       <c r="E16" s="11"/>
     </row>
-    <row r="17" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A17" s="35"/>
       <c r="B17" s="16" t="s">
         <v>102</v>
@@ -2004,7 +2003,7 @@
       </c>
       <c r="E17" s="16"/>
     </row>
-    <row r="18" spans="1:5" ht="81" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="78.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="36"/>
       <c r="B18" s="12" t="s">
         <v>104</v>
@@ -2017,7 +2016,7 @@
       </c>
       <c r="E18" s="13"/>
     </row>
-    <row r="19" spans="1:5" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="29" t="s">
         <v>107</v>
       </c>
@@ -2032,7 +2031,7 @@
       </c>
       <c r="E19" s="28"/>
     </row>
-    <row r="20" spans="1:5" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="29" t="s">
         <v>126</v>
       </c>
@@ -2049,201 +2048,201 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="26"/>
       <c r="C21" s="26"/>
       <c r="D21" s="26"/>
       <c r="E21" s="26"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="26"/>
       <c r="C22" s="26"/>
       <c r="D22" s="26"/>
       <c r="E22" s="26"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="26"/>
       <c r="C23" s="26"/>
       <c r="D23" s="26"/>
       <c r="E23" s="26"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="26"/>
       <c r="C24" s="26"/>
       <c r="D24" s="26"/>
       <c r="E24" s="26"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="26"/>
       <c r="C25" s="26"/>
       <c r="D25" s="26"/>
       <c r="E25" s="26"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="26"/>
       <c r="C26" s="26"/>
       <c r="D26" s="26"/>
       <c r="E26" s="26"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="26"/>
       <c r="C27" s="26"/>
       <c r="D27" s="26"/>
       <c r="E27" s="26"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="26"/>
       <c r="C28" s="26"/>
       <c r="D28" s="26"/>
       <c r="E28" s="26"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="26"/>
       <c r="C29" s="26"/>
       <c r="D29" s="26"/>
       <c r="E29" s="26"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="26"/>
       <c r="C30" s="26"/>
       <c r="D30" s="26"/>
       <c r="E30" s="26"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="26"/>
       <c r="C31" s="26"/>
       <c r="D31" s="26"/>
       <c r="E31" s="26"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="26"/>
       <c r="C32" s="26"/>
       <c r="D32" s="26"/>
       <c r="E32" s="26"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="26"/>
       <c r="C33" s="26"/>
       <c r="D33" s="26"/>
       <c r="E33" s="26"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="26"/>
       <c r="C34" s="26"/>
       <c r="D34" s="26"/>
       <c r="E34" s="26"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="26"/>
       <c r="C35" s="26"/>
       <c r="D35" s="26"/>
       <c r="E35" s="26"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="26"/>
       <c r="C36" s="26"/>
       <c r="D36" s="26"/>
       <c r="E36" s="26"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="26"/>
       <c r="C37" s="26"/>
       <c r="D37" s="26"/>
       <c r="E37" s="26"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="26"/>
       <c r="C38" s="26"/>
       <c r="D38" s="26"/>
       <c r="E38" s="26"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
       <c r="D39" s="26"/>
       <c r="E39" s="26"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="26"/>
       <c r="C40" s="26"/>
       <c r="D40" s="26"/>
       <c r="E40" s="26"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="26"/>
       <c r="C41" s="26"/>
       <c r="D41" s="26"/>
       <c r="E41" s="26"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="26"/>
       <c r="C42" s="26"/>
       <c r="D42" s="26"/>
       <c r="E42" s="26"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="26"/>
       <c r="C43" s="26"/>
       <c r="D43" s="26"/>
       <c r="E43" s="26"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="26"/>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
       <c r="E44" s="26"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="26"/>
       <c r="C45" s="26"/>
       <c r="D45" s="26"/>
       <c r="E45" s="26"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>

</xml_diff>

<commit_message>
Working on the paper tables
</commit_message>
<xml_diff>
--- a/reports/paper_tables.xlsx
+++ b/reports/paper_tables.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Brazel\Dev\cotwins-analyses\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/Dev/cotwins-analyses/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37103DC2-D2D0-2C40-A12C-DE0E9FDC634C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30084" yWindow="456" windowWidth="30084" windowHeight="31764"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30080" windowHeight="31760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="3" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="167">
   <si>
     <t>Type</t>
   </si>
@@ -463,75 +464,21 @@
     <t>HKCS Current user</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>38.0</t>
-  </si>
-  <si>
-    <t>21.2</t>
-  </si>
-  <si>
     <t>Cocaine</t>
   </si>
   <si>
-    <t>5.6</t>
-  </si>
-  <si>
     <t>Heroin</t>
   </si>
   <si>
-    <t>2.0</t>
-  </si>
-  <si>
-    <t>20.0</t>
-  </si>
-  <si>
-    <t>59.2</t>
-  </si>
-  <si>
-    <t>0.9</t>
-  </si>
-  <si>
-    <t>0.0</t>
-  </si>
-  <si>
-    <t>37.9</t>
-  </si>
-  <si>
-    <t>16.6</t>
-  </si>
-  <si>
-    <t>0.4</t>
-  </si>
-  <si>
-    <t>6.4</t>
-  </si>
-  <si>
-    <t>13.3</t>
-  </si>
-  <si>
     <t>HKCS = Healthy Kids Colorado Survey</t>
   </si>
   <si>
-    <t>1.2 (All tobacco)</t>
-  </si>
-  <si>
-    <t>2.1</t>
-  </si>
-  <si>
-    <t>4.5</t>
-  </si>
-  <si>
     <t>Median family income is $100,000-$150,000, Median household income in Colorado is $62,520 (2016 American Community Survey)</t>
   </si>
   <si>
     <t>62.1% of the parents who responded have a bachelor's degree or higher, 38.7% of those 25 years or older in Colorado have a bachelor's degree or higher (2016 American Community Survey)</t>
   </si>
   <si>
-    <t>Dependence in last year</t>
-  </si>
-  <si>
     <t>Maximum age at recruitment = 18, so some loss of oldest high school kids and some 14 year old still in 8th grade</t>
   </si>
   <si>
@@ -539,12 +486,72 @@
   </si>
   <si>
     <t>Must be native born coloradan to be in birth records and in twin registry</t>
+  </si>
+  <si>
+    <t>37.9%</t>
+  </si>
+  <si>
+    <t>16.6%</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>0.9%</t>
+  </si>
+  <si>
+    <t>0.0%</t>
+  </si>
+  <si>
+    <t>59.2%</t>
+  </si>
+  <si>
+    <t>38.0%</t>
+  </si>
+  <si>
+    <t>20.0%</t>
+  </si>
+  <si>
+    <t>5.6%</t>
+  </si>
+  <si>
+    <t>2.0%</t>
+  </si>
+  <si>
+    <t>13.3%</t>
+  </si>
+  <si>
+    <t>6.4%</t>
+  </si>
+  <si>
+    <t>0.4%</t>
+  </si>
+  <si>
+    <t>30.2%</t>
+  </si>
+  <si>
+    <t>21.2%</t>
+  </si>
+  <si>
+    <t>8.6%</t>
+  </si>
+  <si>
+    <t>4.5%</t>
+  </si>
+  <si>
+    <t>2.1%</t>
+  </si>
+  <si>
+    <t>1.2% (All tobacco)</t>
+  </si>
+  <si>
+    <t>Dependent in Last Year</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -570,7 +577,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -763,11 +770,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -879,6 +895,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1192,23 +1209,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.796875" customWidth="1"/>
-    <col min="3" max="3" width="13.69921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>136</v>
       </c>
@@ -1222,138 +1239,141 @@
         <v>138</v>
       </c>
       <c r="F1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>132</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>154</v>
-      </c>
-      <c r="E2" s="33">
-        <v>30.2</v>
+        <v>157</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>160</v>
       </c>
       <c r="F2" s="33" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>133</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>134</v>
       </c>
       <c r="B4" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>139</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="B5" s="33" t="s">
+        <v>150</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>146</v>
       </c>
-      <c r="D4" s="33" t="s">
-        <v>152</v>
-      </c>
-      <c r="E4" s="33">
-        <v>8.6</v>
-      </c>
-      <c r="F4" s="33" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>142</v>
-      </c>
-      <c r="B5" s="33" t="s">
-        <v>148</v>
-      </c>
-      <c r="C5" s="33" t="s">
-        <v>143</v>
-      </c>
-      <c r="D5" s="33" t="s">
-        <v>149</v>
-      </c>
-      <c r="E5" s="33" t="s">
-        <v>139</v>
-      </c>
-      <c r="F5" s="33" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="33" t="s">
-        <v>144</v>
-      </c>
-      <c r="B6" s="33" t="s">
-        <v>149</v>
-      </c>
-      <c r="C6" s="33" t="s">
-        <v>145</v>
-      </c>
-      <c r="D6" s="33" t="s">
-        <v>149</v>
-      </c>
-      <c r="E6" s="33" t="s">
-        <v>139</v>
-      </c>
-      <c r="F6" s="33" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>164</v>
-      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="39"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1361,22 +1381,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1390,7 +1410,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="37" t="s">
         <v>8</v>
       </c>
@@ -1404,7 +1424,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="38"/>
       <c r="B3" s="12" t="s">
         <v>5</v>
@@ -1416,7 +1436,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="34" t="s">
         <v>9</v>
       </c>
@@ -1430,7 +1450,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="35"/>
       <c r="B5" s="4" t="s">
         <v>17</v>
@@ -1442,7 +1462,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="35"/>
       <c r="B6" s="4" t="s">
         <v>13</v>
@@ -1454,7 +1474,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="35"/>
       <c r="B7" s="5" t="s">
         <v>11</v>
@@ -1466,7 +1486,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="35"/>
       <c r="B8" s="5" t="s">
         <v>16</v>
@@ -1478,7 +1498,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="35"/>
       <c r="B9" s="5" t="s">
         <v>15</v>
@@ -1490,7 +1510,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="35"/>
       <c r="B10" s="5" t="s">
         <v>14</v>
@@ -1502,7 +1522,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="35"/>
       <c r="B11" s="32" t="s">
         <v>116</v>
@@ -1514,7 +1534,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36"/>
       <c r="B12" s="6" t="s">
         <v>21</v>
@@ -1526,7 +1546,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="34" t="s">
         <v>24</v>
       </c>
@@ -1540,7 +1560,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="35"/>
       <c r="B14" s="15" t="s">
         <v>26</v>
@@ -1552,7 +1572,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="35"/>
       <c r="B15" s="16" t="s">
         <v>28</v>
@@ -1564,7 +1584,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="35"/>
       <c r="B16" s="16" t="s">
         <v>111</v>
@@ -1576,7 +1596,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="36"/>
       <c r="B17" s="18" t="s">
         <v>31</v>
@@ -1588,7 +1608,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="34" t="s">
         <v>33</v>
       </c>
@@ -1600,7 +1620,7 @@
       </c>
       <c r="D18" s="22"/>
     </row>
-    <row r="19" spans="1:4" ht="31.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="36"/>
       <c r="B19" s="13" t="s">
         <v>36</v>
@@ -1610,7 +1630,7 @@
       </c>
       <c r="D19" s="23"/>
     </row>
-    <row r="20" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="34" t="s">
         <v>38</v>
       </c>
@@ -1624,7 +1644,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="35"/>
       <c r="B21" s="16" t="s">
         <v>40</v>
@@ -1636,7 +1656,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="35"/>
       <c r="B22" s="20" t="s">
         <v>42</v>
@@ -1648,7 +1668,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="35"/>
       <c r="B23" s="15" t="s">
         <v>14</v>
@@ -1660,7 +1680,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A24" s="35"/>
       <c r="B24" s="16" t="s">
         <v>45</v>
@@ -1672,7 +1692,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="35"/>
       <c r="B25" s="15" t="s">
         <v>11</v>
@@ -1684,7 +1704,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="112" x14ac:dyDescent="0.2">
       <c r="A26" s="35"/>
       <c r="B26" s="20" t="s">
         <v>46</v>
@@ -1696,7 +1716,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="35"/>
       <c r="B27" s="16" t="s">
         <v>28</v>
@@ -1708,7 +1728,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="36"/>
       <c r="B28" s="18" t="s">
         <v>48</v>
@@ -1734,23 +1754,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="22.19921875" customWidth="1"/>
-    <col min="3" max="3" width="26.796875" customWidth="1"/>
-    <col min="4" max="4" width="24.296875" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" customWidth="1"/>
+    <col min="3" max="3" width="26.83203125" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1767,7 +1787,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="35" t="s">
         <v>23</v>
       </c>
@@ -1784,7 +1804,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="35"/>
       <c r="B3" s="16" t="s">
         <v>71</v>
@@ -1799,7 +1819,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="35"/>
       <c r="B4" s="16" t="s">
         <v>112</v>
@@ -1814,7 +1834,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="35"/>
       <c r="B5" s="16" t="s">
         <v>75</v>
@@ -1829,7 +1849,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="35"/>
       <c r="B6" s="16" t="s">
         <v>65</v>
@@ -1844,7 +1864,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="35"/>
       <c r="B7" s="16" t="s">
         <v>72</v>
@@ -1859,7 +1879,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="35"/>
       <c r="B8" s="16" t="s">
         <v>77</v>
@@ -1874,7 +1894,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A9" s="35"/>
       <c r="B9" s="16" t="s">
         <v>86</v>
@@ -1889,7 +1909,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" s="35"/>
       <c r="B10" s="16" t="s">
         <v>79</v>
@@ -1904,7 +1924,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="35"/>
       <c r="B11" s="16" t="s">
         <v>82</v>
@@ -1919,7 +1939,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="65" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36"/>
       <c r="B12" s="18" t="s">
         <v>68</v>
@@ -1934,7 +1954,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="34" t="s">
         <v>89</v>
       </c>
@@ -1949,7 +1969,7 @@
       </c>
       <c r="E13" s="27"/>
     </row>
-    <row r="14" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="35"/>
       <c r="B14" s="4" t="s">
         <v>92</v>
@@ -1962,7 +1982,7 @@
       </c>
       <c r="E14" s="16"/>
     </row>
-    <row r="15" spans="1:5" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="36"/>
       <c r="B15" s="12" t="s">
         <v>96</v>
@@ -1975,7 +1995,7 @@
       </c>
       <c r="E15" s="13"/>
     </row>
-    <row r="16" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="34" t="s">
         <v>88</v>
       </c>
@@ -1990,7 +2010,7 @@
       </c>
       <c r="E16" s="11"/>
     </row>
-    <row r="17" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="35"/>
       <c r="B17" s="16" t="s">
         <v>102</v>
@@ -2003,7 +2023,7 @@
       </c>
       <c r="E17" s="16"/>
     </row>
-    <row r="18" spans="1:5" ht="78.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="81" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="36"/>
       <c r="B18" s="12" t="s">
         <v>104</v>
@@ -2016,7 +2036,7 @@
       </c>
       <c r="E18" s="13"/>
     </row>
-    <row r="19" spans="1:5" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
         <v>107</v>
       </c>
@@ -2031,7 +2051,7 @@
       </c>
       <c r="E19" s="28"/>
     </row>
-    <row r="20" spans="1:5" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
         <v>126</v>
       </c>
@@ -2048,201 +2068,201 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="26"/>
       <c r="C21" s="26"/>
       <c r="D21" s="26"/>
       <c r="E21" s="26"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="26"/>
       <c r="C22" s="26"/>
       <c r="D22" s="26"/>
       <c r="E22" s="26"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="26"/>
       <c r="C23" s="26"/>
       <c r="D23" s="26"/>
       <c r="E23" s="26"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="26"/>
       <c r="C24" s="26"/>
       <c r="D24" s="26"/>
       <c r="E24" s="26"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="26"/>
       <c r="C25" s="26"/>
       <c r="D25" s="26"/>
       <c r="E25" s="26"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="26"/>
       <c r="C26" s="26"/>
       <c r="D26" s="26"/>
       <c r="E26" s="26"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="26"/>
       <c r="C27" s="26"/>
       <c r="D27" s="26"/>
       <c r="E27" s="26"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="26"/>
       <c r="C28" s="26"/>
       <c r="D28" s="26"/>
       <c r="E28" s="26"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="26"/>
       <c r="C29" s="26"/>
       <c r="D29" s="26"/>
       <c r="E29" s="26"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="26"/>
       <c r="C30" s="26"/>
       <c r="D30" s="26"/>
       <c r="E30" s="26"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="26"/>
       <c r="C31" s="26"/>
       <c r="D31" s="26"/>
       <c r="E31" s="26"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="26"/>
       <c r="C32" s="26"/>
       <c r="D32" s="26"/>
       <c r="E32" s="26"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="26"/>
       <c r="C33" s="26"/>
       <c r="D33" s="26"/>
       <c r="E33" s="26"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="26"/>
       <c r="C34" s="26"/>
       <c r="D34" s="26"/>
       <c r="E34" s="26"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="26"/>
       <c r="C35" s="26"/>
       <c r="D35" s="26"/>
       <c r="E35" s="26"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="26"/>
       <c r="C36" s="26"/>
       <c r="D36" s="26"/>
       <c r="E36" s="26"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="26"/>
       <c r="C37" s="26"/>
       <c r="D37" s="26"/>
       <c r="E37" s="26"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="26"/>
       <c r="C38" s="26"/>
       <c r="D38" s="26"/>
       <c r="E38" s="26"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
       <c r="D39" s="26"/>
       <c r="E39" s="26"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="26"/>
       <c r="C40" s="26"/>
       <c r="D40" s="26"/>
       <c r="E40" s="26"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="26"/>
       <c r="C41" s="26"/>
       <c r="D41" s="26"/>
       <c r="E41" s="26"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="26"/>
       <c r="C42" s="26"/>
       <c r="D42" s="26"/>
       <c r="E42" s="26"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="26"/>
       <c r="C43" s="26"/>
       <c r="D43" s="26"/>
       <c r="E43" s="26"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="26"/>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
       <c r="E44" s="26"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="B45" s="26"/>
       <c r="C45" s="26"/>
       <c r="D45" s="26"/>
       <c r="E45" s="26"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>

</xml_diff>

<commit_message>
Updating tables for the paper
</commit_message>
<xml_diff>
--- a/reports/paper_tables.xlsx
+++ b/reports/paper_tables.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/Dev/cotwins-analyses/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75CBFC2-AB1C-2240-A7A2-4DC0B3CBDAEC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E8FB2F-CA92-E546-B872-64003AD6550E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30080" windowHeight="31760" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30080" windowHeight="31760" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Table S1" sheetId="1" r:id="rId1"/>
-    <sheet name="Table S2" sheetId="2" r:id="rId2"/>
-    <sheet name="Table S3" sheetId="4" r:id="rId3"/>
-    <sheet name="Table S4" sheetId="3" r:id="rId4"/>
-    <sheet name="Table S5" sheetId="5" r:id="rId5"/>
+    <sheet name="Intake Assessments" sheetId="1" r:id="rId1"/>
+    <sheet name="Follow-Up Assessments" sheetId="2" r:id="rId2"/>
+    <sheet name="Demographics" sheetId="4" r:id="rId3"/>
+    <sheet name="Substance Rates" sheetId="3" r:id="rId4"/>
+    <sheet name="Growth Models" sheetId="5" r:id="rId5"/>
+    <sheet name="Knot Point Models" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="368">
   <si>
     <t>Type</t>
   </si>
@@ -1019,6 +1021,138 @@
   </si>
   <si>
     <t>0.299</t>
+  </si>
+  <si>
+    <t>Slope1</t>
+  </si>
+  <si>
+    <t>Slope2</t>
+  </si>
+  <si>
+    <t>Fixed Knot Point</t>
+  </si>
+  <si>
+    <t>Dynamic Knot Point</t>
+  </si>
+  <si>
+    <t>8303.0</t>
+  </si>
+  <si>
+    <t>8223.4</t>
+  </si>
+  <si>
+    <t>8207.3</t>
+  </si>
+  <si>
+    <t>&lt;2.2E-16</t>
+  </si>
+  <si>
+    <t>0.051</t>
+  </si>
+  <si>
+    <t>0.283</t>
+  </si>
+  <si>
+    <t>0.250</t>
+  </si>
+  <si>
+    <t>0.049</t>
+  </si>
+  <si>
+    <t>2.54E-6</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>0.069</t>
+  </si>
+  <si>
+    <t>0.044</t>
+  </si>
+  <si>
+    <t>0.118</t>
+  </si>
+  <si>
+    <t>0.219</t>
+  </si>
+  <si>
+    <t>1.23E-4</t>
+  </si>
+  <si>
+    <t>0.108</t>
+  </si>
+  <si>
+    <t>0.124</t>
+  </si>
+  <si>
+    <t>0.390</t>
+  </si>
+  <si>
+    <t>0.062</t>
+  </si>
+  <si>
+    <t>0.152</t>
+  </si>
+  <si>
+    <t>0.233</t>
+  </si>
+  <si>
+    <t>0.050</t>
+  </si>
+  <si>
+    <t>1.35E-5</t>
+  </si>
+  <si>
+    <t>0.104</t>
+  </si>
+  <si>
+    <t>0.133</t>
+  </si>
+  <si>
+    <t>0.435</t>
+  </si>
+  <si>
+    <t>-23.24</t>
+  </si>
+  <si>
+    <t>-344.69</t>
+  </si>
+  <si>
+    <t>-270.27</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0.084</t>
+  </si>
+  <si>
+    <t>0.042</t>
+  </si>
+  <si>
+    <t>0.110</t>
+  </si>
+  <si>
+    <t>0.041</t>
+  </si>
+  <si>
+    <t>0.404</t>
+  </si>
+  <si>
+    <t>0.083</t>
+  </si>
+  <si>
+    <t>0.564</t>
+  </si>
+  <si>
+    <t>0.032</t>
+  </si>
+  <si>
+    <t>0.085</t>
+  </si>
+  <si>
+    <t>0.703</t>
   </si>
 </sst>
 </file>
@@ -1354,6 +1488,7 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1369,11 +1504,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1719,7 +1853,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="39" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="10" t="s">
@@ -1733,7 +1867,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="39"/>
+      <c r="A3" s="40"/>
       <c r="B3" s="12" t="s">
         <v>5</v>
       </c>
@@ -1745,7 +1879,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="36" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -1759,7 +1893,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A5" s="36"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="4" t="s">
         <v>17</v>
       </c>
@@ -1771,7 +1905,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A6" s="36"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
@@ -1783,7 +1917,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="36"/>
+      <c r="A7" s="37"/>
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
@@ -1795,7 +1929,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" s="36"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="5" t="s">
         <v>16</v>
       </c>
@@ -1807,7 +1941,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A9" s="36"/>
+      <c r="A9" s="37"/>
       <c r="B9" s="5" t="s">
         <v>15</v>
       </c>
@@ -1819,7 +1953,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A10" s="36"/>
+      <c r="A10" s="37"/>
       <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
@@ -1831,7 +1965,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A11" s="36"/>
+      <c r="A11" s="37"/>
       <c r="B11" s="32" t="s">
         <v>116</v>
       </c>
@@ -1843,7 +1977,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="37"/>
+      <c r="A12" s="38"/>
       <c r="B12" s="6" t="s">
         <v>21</v>
       </c>
@@ -1855,7 +1989,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="36" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="17" t="s">
@@ -1869,7 +2003,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A14" s="36"/>
+      <c r="A14" s="37"/>
       <c r="B14" s="15" t="s">
         <v>26</v>
       </c>
@@ -1881,7 +2015,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="36"/>
+      <c r="A15" s="37"/>
       <c r="B15" s="16" t="s">
         <v>28</v>
       </c>
@@ -1893,7 +2027,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A16" s="36"/>
+      <c r="A16" s="37"/>
       <c r="B16" s="16" t="s">
         <v>111</v>
       </c>
@@ -1905,7 +2039,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="37"/>
+      <c r="A17" s="38"/>
       <c r="B17" s="18" t="s">
         <v>31</v>
       </c>
@@ -1917,7 +2051,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="36" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="20" t="s">
@@ -1929,7 +2063,7 @@
       <c r="D18" s="22"/>
     </row>
     <row r="19" spans="1:4" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="37"/>
+      <c r="A19" s="38"/>
       <c r="B19" s="13" t="s">
         <v>36</v>
       </c>
@@ -1939,7 +2073,7 @@
       <c r="D19" s="23"/>
     </row>
     <row r="20" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="36" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="11" t="s">
@@ -1953,7 +2087,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A21" s="36"/>
+      <c r="A21" s="37"/>
       <c r="B21" s="16" t="s">
         <v>40</v>
       </c>
@@ -1965,7 +2099,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="36"/>
+      <c r="A22" s="37"/>
       <c r="B22" s="20" t="s">
         <v>42</v>
       </c>
@@ -1977,7 +2111,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A23" s="36"/>
+      <c r="A23" s="37"/>
       <c r="B23" s="15" t="s">
         <v>14</v>
       </c>
@@ -1989,7 +2123,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A24" s="36"/>
+      <c r="A24" s="37"/>
       <c r="B24" s="16" t="s">
         <v>45</v>
       </c>
@@ -2001,7 +2135,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A25" s="36"/>
+      <c r="A25" s="37"/>
       <c r="B25" s="15" t="s">
         <v>11</v>
       </c>
@@ -2013,7 +2147,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="112" x14ac:dyDescent="0.2">
-      <c r="A26" s="36"/>
+      <c r="A26" s="37"/>
       <c r="B26" s="20" t="s">
         <v>46</v>
       </c>
@@ -2025,7 +2159,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="36"/>
+      <c r="A27" s="37"/>
       <c r="B27" s="16" t="s">
         <v>28</v>
       </c>
@@ -2037,7 +2171,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="37"/>
+      <c r="A28" s="38"/>
       <c r="B28" s="18" t="s">
         <v>48</v>
       </c>
@@ -2096,7 +2230,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="37" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="11" t="s">
@@ -2113,7 +2247,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A3" s="36"/>
+      <c r="A3" s="37"/>
       <c r="B3" s="16" t="s">
         <v>71</v>
       </c>
@@ -2128,7 +2262,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A4" s="36"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="16" t="s">
         <v>112</v>
       </c>
@@ -2143,7 +2277,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A5" s="36"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="16" t="s">
         <v>75</v>
       </c>
@@ -2158,7 +2292,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A6" s="36"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="16" t="s">
         <v>65</v>
       </c>
@@ -2173,7 +2307,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="36"/>
+      <c r="A7" s="37"/>
       <c r="B7" s="16" t="s">
         <v>72</v>
       </c>
@@ -2188,7 +2322,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A8" s="36"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="16" t="s">
         <v>77</v>
       </c>
@@ -2203,7 +2337,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A9" s="36"/>
+      <c r="A9" s="37"/>
       <c r="B9" s="16" t="s">
         <v>86</v>
       </c>
@@ -2218,7 +2352,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A10" s="36"/>
+      <c r="A10" s="37"/>
       <c r="B10" s="16" t="s">
         <v>79</v>
       </c>
@@ -2233,7 +2367,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A11" s="36"/>
+      <c r="A11" s="37"/>
       <c r="B11" s="16" t="s">
         <v>82</v>
       </c>
@@ -2248,7 +2382,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="37"/>
+      <c r="A12" s="38"/>
       <c r="B12" s="18" t="s">
         <v>68</v>
       </c>
@@ -2263,7 +2397,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="36" t="s">
         <v>89</v>
       </c>
       <c r="B13" s="27" t="s">
@@ -2278,7 +2412,7 @@
       <c r="E13" s="27"/>
     </row>
     <row r="14" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A14" s="36"/>
+      <c r="A14" s="37"/>
       <c r="B14" s="4" t="s">
         <v>92</v>
       </c>
@@ -2291,7 +2425,7 @@
       <c r="E14" s="16"/>
     </row>
     <row r="15" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="37"/>
+      <c r="A15" s="38"/>
       <c r="B15" s="12" t="s">
         <v>96</v>
       </c>
@@ -2304,7 +2438,7 @@
       <c r="E15" s="13"/>
     </row>
     <row r="16" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="36" t="s">
         <v>88</v>
       </c>
       <c r="B16" s="11" t="s">
@@ -2319,7 +2453,7 @@
       <c r="E16" s="11"/>
     </row>
     <row r="17" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A17" s="36"/>
+      <c r="A17" s="37"/>
       <c r="B17" s="16" t="s">
         <v>102</v>
       </c>
@@ -2332,7 +2466,7 @@
       <c r="E17" s="16"/>
     </row>
     <row r="18" spans="1:5" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="37"/>
+      <c r="A18" s="38"/>
       <c r="B18" s="12" t="s">
         <v>104</v>
       </c>
@@ -2875,7 +3009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{174D37A8-7E1D-8840-9C3F-74515625221D}">
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -2885,74 +3019,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="40"/>
-      <c r="B1" s="40"/>
-      <c r="C1" s="42" t="s">
+      <c r="A1" s="35"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="41" t="s">
         <v>201</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="41" t="s">
+      <c r="D1" s="41"/>
+      <c r="E1" s="42" t="s">
         <v>207</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="35" t="s">
         <v>193</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="35" t="s">
         <v>194</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="35" t="s">
         <v>200</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="35" t="s">
         <v>202</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="35" t="s">
         <v>203</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="G2" s="40" t="s">
+      <c r="G2" s="35" t="s">
         <v>202</v>
       </c>
-      <c r="H2" s="40" t="s">
+      <c r="H2" s="35" t="s">
         <v>205</v>
       </c>
-      <c r="I2" s="40" t="s">
+      <c r="I2" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="J2" s="40" t="s">
+      <c r="J2" s="35" t="s">
         <v>202</v>
       </c>
-      <c r="K2" s="40" t="s">
+      <c r="K2" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="L2" s="40" t="s">
+      <c r="L2" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="M2" s="40" t="s">
+      <c r="M2" s="35" t="s">
         <v>202</v>
       </c>
-      <c r="N2" s="40" t="s">
+      <c r="N2" s="35" t="s">
         <v>206</v>
       </c>
-      <c r="O2" s="40" t="s">
+      <c r="O2" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="P2" s="40" t="s">
+      <c r="P2" s="35" t="s">
         <v>202</v>
       </c>
     </row>
@@ -3534,4 +3668,359 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDE6952F-B094-AC4C-9C01-A81131620637}">
+  <dimension ref="A1:P10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8:M8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H1" t="s">
+        <v>324</v>
+      </c>
+      <c r="I1" t="s">
+        <v>204</v>
+      </c>
+      <c r="J1" t="s">
+        <v>202</v>
+      </c>
+      <c r="K1" t="s">
+        <v>325</v>
+      </c>
+      <c r="L1" t="s">
+        <v>204</v>
+      </c>
+      <c r="M1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>328</v>
+      </c>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33" t="s">
+        <v>332</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>290</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>333</v>
+      </c>
+      <c r="H2" s="33" t="s">
+        <v>334</v>
+      </c>
+      <c r="I2" s="33" t="s">
+        <v>335</v>
+      </c>
+      <c r="J2" s="33" t="s">
+        <v>336</v>
+      </c>
+      <c r="K2" s="33" t="s">
+        <v>337</v>
+      </c>
+      <c r="L2" s="33" t="s">
+        <v>337</v>
+      </c>
+      <c r="M2" s="33" t="s">
+        <v>337</v>
+      </c>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>329</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>331</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>338</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>339</v>
+      </c>
+      <c r="G3" s="33" t="s">
+        <v>340</v>
+      </c>
+      <c r="H3" s="33" t="s">
+        <v>341</v>
+      </c>
+      <c r="I3" s="33" t="s">
+        <v>225</v>
+      </c>
+      <c r="J3" s="33" t="s">
+        <v>342</v>
+      </c>
+      <c r="K3" s="33" t="s">
+        <v>343</v>
+      </c>
+      <c r="L3" s="33" t="s">
+        <v>344</v>
+      </c>
+      <c r="M3" s="33" t="s">
+        <v>345</v>
+      </c>
+      <c r="N3" s="33"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>327</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>330</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>331</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>346</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>267</v>
+      </c>
+      <c r="G4" s="33" t="s">
+        <v>347</v>
+      </c>
+      <c r="H4" s="33" t="s">
+        <v>348</v>
+      </c>
+      <c r="I4" s="33" t="s">
+        <v>349</v>
+      </c>
+      <c r="J4" s="33" t="s">
+        <v>350</v>
+      </c>
+      <c r="K4" s="33" t="s">
+        <v>351</v>
+      </c>
+      <c r="L4" s="33" t="s">
+        <v>352</v>
+      </c>
+      <c r="M4" s="33" t="s">
+        <v>353</v>
+      </c>
+      <c r="N4" s="33"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="33"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>354</v>
+      </c>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33" t="s">
+        <v>358</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>359</v>
+      </c>
+      <c r="G5" s="33" t="s">
+        <v>349</v>
+      </c>
+      <c r="H5" s="33" t="s">
+        <v>349</v>
+      </c>
+      <c r="I5" s="33" t="s">
+        <v>265</v>
+      </c>
+      <c r="J5" s="33" t="s">
+        <v>360</v>
+      </c>
+      <c r="K5" s="33" t="s">
+        <v>337</v>
+      </c>
+      <c r="L5" s="33" t="s">
+        <v>337</v>
+      </c>
+      <c r="M5" s="33" t="s">
+        <v>337</v>
+      </c>
+      <c r="N5" s="33"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="33"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>326</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>355</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>331</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>241</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>267</v>
+      </c>
+      <c r="G6" s="33" t="s">
+        <v>361</v>
+      </c>
+      <c r="H6" s="33" t="s">
+        <v>359</v>
+      </c>
+      <c r="I6" s="33" t="s">
+        <v>349</v>
+      </c>
+      <c r="J6" s="33" t="s">
+        <v>362</v>
+      </c>
+      <c r="K6" s="33" t="s">
+        <v>290</v>
+      </c>
+      <c r="L6" s="33" t="s">
+        <v>363</v>
+      </c>
+      <c r="M6" s="33" t="s">
+        <v>364</v>
+      </c>
+      <c r="N6" s="33"/>
+      <c r="O6" s="33"/>
+      <c r="P6" s="33"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>327</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>356</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>357</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>267</v>
+      </c>
+      <c r="G7" s="33" t="s">
+        <v>267</v>
+      </c>
+      <c r="H7" s="33" t="s">
+        <v>359</v>
+      </c>
+      <c r="I7" s="33" t="s">
+        <v>267</v>
+      </c>
+      <c r="J7" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="K7" s="33" t="s">
+        <v>365</v>
+      </c>
+      <c r="L7" s="33" t="s">
+        <v>366</v>
+      </c>
+      <c r="M7" s="33" t="s">
+        <v>367</v>
+      </c>
+      <c r="N7" s="33"/>
+      <c r="O7" s="33"/>
+      <c r="P7" s="33"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="33"/>
+      <c r="O8" s="33"/>
+      <c r="P8" s="33"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="33"/>
+      <c r="O9" s="33"/>
+      <c r="P9" s="33"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="33"/>
+      <c r="O10" s="33"/>
+      <c r="P10" s="33"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>